<commit_message>
Site updated: 2020-06-18 10:33:22
</commit_message>
<xml_diff>
--- a/2020/06/15/2020春招-FLAG面试频率最高的100道题/2020春招-FLAG面试频率最高的100道题.xlsx
+++ b/2020/06/15/2020春招-FLAG面试频率最高的100道题/2020春招-FLAG面试频率最高的100道题.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1644b6d277bbd0f5/文档/Louis' Blog/source/_drafts/2020春招-FLAG面试频率最高的100道题/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_247634D3317F434A46BAEF313E0FE89AAB6DB088" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C53E01A2-4EC9-466C-AA44-2A9BB7F2BFC8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="2168" yWindow="1868" windowWidth="15389" windowHeight="9644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -729,8 +735,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,7 +826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,6 +842,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +884,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,8 +912,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -913,6 +928,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,6 +951,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1195,32 +1216,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.875" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="11.375" customWidth="1"/>
-    <col min="4" max="4" width="40.25" customWidth="1"/>
-    <col min="5" max="5" width="107.625" customWidth="1"/>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
+    <col min="2" max="2" width="15.46484375" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
+    <col min="4" max="4" width="40.265625" customWidth="1"/>
+    <col min="5" max="5" width="107.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.1" customHeight="1">
+    <row r="1" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1235,148 +1256,148 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75">
+    <row r="4" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75">
+    <row r="5" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75">
+    <row r="6" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="18.75">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="18.75">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75">
+    <row r="9" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75">
+    <row r="10" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="6" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75">
+    <row r="11" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75">
+    <row r="12" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75">
+    <row r="13" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75">
+    <row r="14" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.75">
+    <row r="15" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1384,10 +1405,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18.75">
+    <row r="16" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1395,10 +1416,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="6" t="s">
         <v>20</v>
       </c>
@@ -1406,10 +1427,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
@@ -1417,10 +1438,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1428,10 +1449,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1">
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1439,10 +1460,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1">
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="6" t="s">
         <v>41</v>
       </c>
@@ -1450,10 +1471,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="6" t="s">
         <v>43</v>
       </c>
@@ -1461,10 +1482,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1">
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1474,10 +1495,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1">
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="6" t="s">
         <v>26</v>
       </c>
@@ -1485,10 +1506,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1">
+    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="5" t="s">
         <v>54</v>
       </c>
@@ -1496,10 +1517,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1">
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="5" t="s">
         <v>47</v>
       </c>
@@ -1507,10 +1528,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1">
+    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="5" t="s">
         <v>55</v>
       </c>
@@ -1518,12 +1539,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1533,9 +1554,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75">
-      <c r="B29" s="11"/>
-      <c r="C29" s="10"/>
+    <row r="29" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B29" s="12"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="4" t="s">
         <v>58</v>
       </c>
@@ -1543,9 +1564,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75">
-      <c r="B30" s="11"/>
-      <c r="C30" s="10"/>
+    <row r="30" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B30" s="12"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1553,9 +1574,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.75">
-      <c r="B31" s="11"/>
-      <c r="C31" s="10"/>
+    <row r="31" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B31" s="12"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="5" t="s">
         <v>60</v>
       </c>
@@ -1563,9 +1584,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75">
-      <c r="B32" s="11"/>
-      <c r="C32" s="10"/>
+    <row r="32" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B32" s="12"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="5" t="s">
         <v>61</v>
       </c>
@@ -1573,9 +1594,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="18.75">
-      <c r="B33" s="11"/>
-      <c r="C33" s="10"/>
+    <row r="33" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B33" s="12"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="5" t="s">
         <v>66</v>
       </c>
@@ -1583,9 +1604,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="18.75">
-      <c r="B34" s="11"/>
-      <c r="C34" s="9" t="s">
+    <row r="34" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B34" s="12"/>
+      <c r="C34" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -1595,9 +1616,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="18.75">
-      <c r="B35" s="11"/>
-      <c r="C35" s="9"/>
+    <row r="35" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B35" s="12"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="6" t="s">
         <v>68</v>
       </c>
@@ -1605,9 +1626,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="18.75">
-      <c r="B36" s="11"/>
-      <c r="C36" s="9"/>
+    <row r="36" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B36" s="12"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="5" t="s">
         <v>69</v>
       </c>
@@ -1615,9 +1636,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="18.75">
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
+    <row r="37" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B37" s="12"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="6" t="s">
         <v>70</v>
       </c>
@@ -1625,9 +1646,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="18.75">
-      <c r="B38" s="11"/>
-      <c r="C38" s="9"/>
+    <row r="38" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B38" s="12"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="6" t="s">
         <v>71</v>
       </c>
@@ -1635,9 +1656,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="18.75">
-      <c r="B39" s="11"/>
-      <c r="C39" s="9"/>
+    <row r="39" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B39" s="12"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="5" t="s">
         <v>72</v>
       </c>
@@ -1645,9 +1666,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="18.75">
-      <c r="B40" s="11"/>
-      <c r="C40" s="9"/>
+    <row r="40" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B40" s="12"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="6" t="s">
         <v>73</v>
       </c>
@@ -1655,9 +1676,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="18.75">
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
+    <row r="41" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B41" s="12"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="6" t="s">
         <v>74</v>
       </c>
@@ -1665,9 +1686,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="18.75">
-      <c r="B42" s="11"/>
-      <c r="C42" s="9"/>
+    <row r="42" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B42" s="12"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="6" t="s">
         <v>75</v>
       </c>
@@ -1675,9 +1696,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="18.75">
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
+    <row r="43" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B43" s="12"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="6" t="s">
         <v>76</v>
       </c>
@@ -1685,9 +1706,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="18.75">
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
+    <row r="44" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B44" s="12"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="6" t="s">
         <v>77</v>
       </c>
@@ -1695,9 +1716,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="18.75">
-      <c r="B45" s="11"/>
-      <c r="C45" s="9"/>
+    <row r="45" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B45" s="12"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="6" t="s">
         <v>78</v>
       </c>
@@ -1705,9 +1726,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="18.75">
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
+    <row r="46" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B46" s="12"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="5" t="s">
         <v>79</v>
       </c>
@@ -1715,9 +1736,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="18.75">
-      <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
+    <row r="47" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B47" s="12"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="5" t="s">
         <v>80</v>
       </c>
@@ -1725,9 +1746,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="18.75">
-      <c r="B48" s="11"/>
-      <c r="C48" s="9"/>
+    <row r="48" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B48" s="12"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="5" t="s">
         <v>81</v>
       </c>
@@ -1735,9 +1756,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="18.75">
-      <c r="B49" s="11"/>
-      <c r="C49" s="10" t="s">
+    <row r="49" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B49" s="12"/>
+      <c r="C49" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -1747,9 +1768,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="18.75">
-      <c r="B50" s="11"/>
-      <c r="C50" s="10"/>
+    <row r="50" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B50" s="12"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="6" t="s">
         <v>84</v>
       </c>
@@ -1757,9 +1778,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="18.75">
-      <c r="B51" s="11"/>
-      <c r="C51" s="10"/>
+    <row r="51" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B51" s="12"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="5" t="s">
         <v>86</v>
       </c>
@@ -1767,9 +1788,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="18.75">
-      <c r="B52" s="11"/>
-      <c r="C52" s="10"/>
+    <row r="52" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B52" s="12"/>
+      <c r="C52" s="11"/>
       <c r="D52" s="5" t="s">
         <v>88</v>
       </c>
@@ -1777,11 +1798,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="18.75">
-      <c r="B53" s="11" t="s">
+    <row r="53" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B53" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -1791,9 +1812,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="18.75">
-      <c r="B54" s="11"/>
-      <c r="C54" s="10"/>
+    <row r="54" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B54" s="12"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="4" t="s">
         <v>114</v>
       </c>
@@ -1801,9 +1822,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="18.75">
-      <c r="B55" s="11"/>
-      <c r="C55" s="10"/>
+    <row r="55" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B55" s="12"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="5" t="s">
         <v>116</v>
       </c>
@@ -1811,9 +1832,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="18.75">
-      <c r="B56" s="11"/>
-      <c r="C56" s="10"/>
+    <row r="56" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B56" s="12"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="6" t="s">
         <v>118</v>
       </c>
@@ -1821,9 +1842,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="18.75">
-      <c r="B57" s="11"/>
-      <c r="C57" s="10"/>
+    <row r="57" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B57" s="12"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="6" t="s">
         <v>120</v>
       </c>
@@ -1831,9 +1852,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="18.75">
-      <c r="B58" s="11"/>
-      <c r="C58" s="10"/>
+    <row r="58" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B58" s="12"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="5" t="s">
         <v>122</v>
       </c>
@@ -1841,9 +1862,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="18.75">
-      <c r="B59" s="11"/>
-      <c r="C59" s="10"/>
+    <row r="59" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B59" s="12"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="6" t="s">
         <v>58</v>
       </c>
@@ -1851,9 +1872,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="18.75">
-      <c r="B60" s="11"/>
-      <c r="C60" s="10"/>
+    <row r="60" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B60" s="12"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="6" t="s">
         <v>124</v>
       </c>
@@ -1861,9 +1882,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="18.75">
-      <c r="B61" s="11"/>
-      <c r="C61" s="10"/>
+    <row r="61" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B61" s="12"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="5" t="s">
         <v>126</v>
       </c>
@@ -1871,9 +1892,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="18.75">
-      <c r="B62" s="11"/>
-      <c r="C62" s="10"/>
+    <row r="62" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B62" s="12"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="5" t="s">
         <v>128</v>
       </c>
@@ -1881,9 +1902,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="18.75">
-      <c r="B63" s="11"/>
-      <c r="C63" s="9" t="s">
+    <row r="63" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B63" s="12"/>
+      <c r="C63" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="6" t="s">
@@ -1893,9 +1914,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="18.75">
-      <c r="B64" s="11"/>
-      <c r="C64" s="9"/>
+    <row r="64" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B64" s="12"/>
+      <c r="C64" s="15"/>
       <c r="D64" s="6" t="s">
         <v>132</v>
       </c>
@@ -1903,9 +1924,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="18.75">
-      <c r="B65" s="11"/>
-      <c r="C65" s="9"/>
+    <row r="65" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B65" s="12"/>
+      <c r="C65" s="15"/>
       <c r="D65" s="5" t="s">
         <v>134</v>
       </c>
@@ -1913,9 +1934,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="18.75">
-      <c r="B66" s="11"/>
-      <c r="C66" s="9"/>
+    <row r="66" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B66" s="12"/>
+      <c r="C66" s="15"/>
       <c r="D66" s="6" t="s">
         <v>136</v>
       </c>
@@ -1923,9 +1944,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="18.75">
-      <c r="B67" s="11"/>
-      <c r="C67" s="9"/>
+    <row r="67" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B67" s="12"/>
+      <c r="C67" s="15"/>
       <c r="D67" s="6" t="s">
         <v>138</v>
       </c>
@@ -1933,9 +1954,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="18.75">
-      <c r="B68" s="11"/>
-      <c r="C68" s="9"/>
+    <row r="68" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B68" s="12"/>
+      <c r="C68" s="15"/>
       <c r="D68" s="5" t="s">
         <v>140</v>
       </c>
@@ -1943,9 +1964,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="18.75">
-      <c r="B69" s="11"/>
-      <c r="C69" s="9"/>
+    <row r="69" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B69" s="12"/>
+      <c r="C69" s="15"/>
       <c r="D69" s="6" t="s">
         <v>142</v>
       </c>
@@ -1953,9 +1974,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="18.75">
-      <c r="B70" s="11"/>
-      <c r="C70" s="9"/>
+    <row r="70" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B70" s="12"/>
+      <c r="C70" s="15"/>
       <c r="D70" s="6" t="s">
         <v>144</v>
       </c>
@@ -1963,9 +1984,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="18.75">
-      <c r="B71" s="11"/>
-      <c r="C71" s="9"/>
+    <row r="71" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B71" s="12"/>
+      <c r="C71" s="15"/>
       <c r="D71" s="6" t="s">
         <v>146</v>
       </c>
@@ -1973,9 +1994,9 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="2:5" ht="18.75">
-      <c r="B72" s="11"/>
-      <c r="C72" s="9"/>
+    <row r="72" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B72" s="12"/>
+      <c r="C72" s="15"/>
       <c r="D72" s="6" t="s">
         <v>148</v>
       </c>
@@ -1983,9 +2004,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="2:5" ht="18.75">
-      <c r="B73" s="11"/>
-      <c r="C73" s="10" t="s">
+    <row r="73" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B73" s="12"/>
+      <c r="C73" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D73" s="6" t="s">
@@ -1995,9 +2016,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="2:5" ht="18.75">
-      <c r="B74" s="11"/>
-      <c r="C74" s="10"/>
+    <row r="74" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B74" s="12"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="6" t="s">
         <v>152</v>
       </c>
@@ -2005,9 +2026,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:5" ht="18.75">
-      <c r="B75" s="11"/>
-      <c r="C75" s="10"/>
+    <row r="75" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B75" s="12"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="5" t="s">
         <v>153</v>
       </c>
@@ -2015,9 +2036,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="18.75">
-      <c r="B76" s="11"/>
-      <c r="C76" s="10"/>
+    <row r="76" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B76" s="12"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="5" t="s">
         <v>155</v>
       </c>
@@ -2025,9 +2046,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="18.75">
-      <c r="B77" s="11"/>
-      <c r="C77" s="10"/>
+    <row r="77" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B77" s="12"/>
+      <c r="C77" s="11"/>
       <c r="D77" s="5" t="s">
         <v>157</v>
       </c>
@@ -2035,11 +2056,11 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="2:5" ht="18.75">
-      <c r="B78" s="11" t="s">
+    <row r="78" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B78" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -2049,9 +2070,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="18.75">
-      <c r="B79" s="11"/>
-      <c r="C79" s="10"/>
+    <row r="79" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B79" s="12"/>
+      <c r="C79" s="11"/>
       <c r="D79" s="4" t="s">
         <v>114</v>
       </c>
@@ -2059,9 +2080,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="2:5" ht="18.75">
-      <c r="B80" s="11"/>
-      <c r="C80" s="10"/>
+    <row r="80" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B80" s="12"/>
+      <c r="C80" s="11"/>
       <c r="D80" s="5" t="s">
         <v>39</v>
       </c>
@@ -2069,9 +2090,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="18.75">
-      <c r="B81" s="11"/>
-      <c r="C81" s="10"/>
+    <row r="81" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B81" s="12"/>
+      <c r="C81" s="11"/>
       <c r="D81" s="6" t="s">
         <v>62</v>
       </c>
@@ -2079,9 +2100,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="82" spans="2:5" ht="18.75">
-      <c r="B82" s="11"/>
-      <c r="C82" s="10"/>
+    <row r="82" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B82" s="12"/>
+      <c r="C82" s="11"/>
       <c r="D82" s="6" t="s">
         <v>124</v>
       </c>
@@ -2089,9 +2110,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="2:5" ht="18.75">
-      <c r="B83" s="11"/>
-      <c r="C83" s="9" t="s">
+    <row r="83" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B83" s="12"/>
+      <c r="C83" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D83" s="6" t="s">
@@ -2101,9 +2122,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="18.75">
-      <c r="B84" s="11"/>
-      <c r="C84" s="9"/>
+    <row r="84" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B84" s="12"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="6" t="s">
         <v>130</v>
       </c>
@@ -2111,9 +2132,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="18.75">
-      <c r="B85" s="11"/>
-      <c r="C85" s="9"/>
+    <row r="85" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B85" s="12"/>
+      <c r="C85" s="15"/>
       <c r="D85" s="5" t="s">
         <v>134</v>
       </c>
@@ -2121,9 +2142,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="2:5" ht="18.75">
-      <c r="B86" s="11"/>
-      <c r="C86" s="9"/>
+    <row r="86" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B86" s="12"/>
+      <c r="C86" s="15"/>
       <c r="D86" s="6" t="s">
         <v>166</v>
       </c>
@@ -2131,9 +2152,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="18.75">
-      <c r="B87" s="11"/>
-      <c r="C87" s="9"/>
+    <row r="87" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B87" s="12"/>
+      <c r="C87" s="15"/>
       <c r="D87" s="6" t="s">
         <v>168</v>
       </c>
@@ -2141,9 +2162,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="2:5" ht="18.75">
-      <c r="B88" s="11"/>
-      <c r="C88" s="9"/>
+    <row r="88" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B88" s="12"/>
+      <c r="C88" s="15"/>
       <c r="D88" s="5" t="s">
         <v>170</v>
       </c>
@@ -2151,9 +2172,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="2:5" ht="18.75">
-      <c r="B89" s="11"/>
-      <c r="C89" s="9"/>
+    <row r="89" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B89" s="12"/>
+      <c r="C89" s="15"/>
       <c r="D89" s="6" t="s">
         <v>142</v>
       </c>
@@ -2161,9 +2182,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="2:5" ht="18.75">
-      <c r="B90" s="11"/>
-      <c r="C90" s="9"/>
+    <row r="90" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B90" s="12"/>
+      <c r="C90" s="15"/>
       <c r="D90" s="6" t="s">
         <v>172</v>
       </c>
@@ -2171,9 +2192,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="2:5" ht="18.75">
-      <c r="B91" s="11"/>
-      <c r="C91" s="9"/>
+    <row r="91" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B91" s="12"/>
+      <c r="C91" s="15"/>
       <c r="D91" s="6" t="s">
         <v>176</v>
       </c>
@@ -2181,9 +2202,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="2:5" ht="18.75">
-      <c r="B92" s="11"/>
-      <c r="C92" s="9"/>
+    <row r="92" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B92" s="12"/>
+      <c r="C92" s="15"/>
       <c r="D92" s="6" t="s">
         <v>178</v>
       </c>
@@ -2191,9 +2212,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="2:5" ht="18.75">
-      <c r="B93" s="11"/>
-      <c r="C93" s="9"/>
+    <row r="93" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B93" s="12"/>
+      <c r="C93" s="15"/>
       <c r="D93" s="5" t="s">
         <v>180</v>
       </c>
@@ -2201,9 +2222,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="2:5" ht="18.75">
-      <c r="B94" s="11"/>
-      <c r="C94" s="9"/>
+    <row r="94" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B94" s="12"/>
+      <c r="C94" s="15"/>
       <c r="D94" s="6" t="s">
         <v>174</v>
       </c>
@@ -2211,9 +2232,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="2:5" ht="18.75">
-      <c r="B95" s="11"/>
-      <c r="C95" s="9"/>
+    <row r="95" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B95" s="12"/>
+      <c r="C95" s="15"/>
       <c r="D95" s="6" t="s">
         <v>182</v>
       </c>
@@ -2221,9 +2242,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="2:5" ht="18.75">
-      <c r="B96" s="11"/>
-      <c r="C96" s="9"/>
+    <row r="96" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B96" s="12"/>
+      <c r="C96" s="15"/>
       <c r="D96" s="6" t="s">
         <v>184</v>
       </c>
@@ -2231,9 +2252,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="2:5" ht="18.75">
-      <c r="B97" s="11"/>
-      <c r="C97" s="9"/>
+    <row r="97" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B97" s="12"/>
+      <c r="C97" s="15"/>
       <c r="D97" s="5" t="s">
         <v>186</v>
       </c>
@@ -2241,9 +2262,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="2:5" ht="18.75">
-      <c r="B98" s="11"/>
-      <c r="C98" s="10" t="s">
+    <row r="98" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B98" s="12"/>
+      <c r="C98" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -2253,9 +2274,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="2:5" ht="18.75">
-      <c r="B99" s="11"/>
-      <c r="C99" s="10"/>
+    <row r="99" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B99" s="12"/>
+      <c r="C99" s="11"/>
       <c r="D99" s="6" t="s">
         <v>188</v>
       </c>
@@ -2263,9 +2284,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="2:5" ht="18.75">
-      <c r="B100" s="11"/>
-      <c r="C100" s="10"/>
+    <row r="100" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B100" s="12"/>
+      <c r="C100" s="11"/>
       <c r="D100" s="5" t="s">
         <v>190</v>
       </c>
@@ -2273,9 +2294,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="2:5" ht="18.75">
-      <c r="B101" s="11"/>
-      <c r="C101" s="10"/>
+    <row r="101" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B101" s="12"/>
+      <c r="C101" s="11"/>
       <c r="D101" s="5" t="s">
         <v>192</v>
       </c>
@@ -2283,9 +2304,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="102" spans="2:5" ht="18.75">
-      <c r="B102" s="11"/>
-      <c r="C102" s="10"/>
+    <row r="102" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
+      <c r="B102" s="12"/>
+      <c r="C102" s="11"/>
       <c r="D102" s="5" t="s">
         <v>195</v>
       </c>
@@ -2303,118 +2324,118 @@
     <mergeCell ref="C78:C82"/>
     <mergeCell ref="C83:C97"/>
     <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B3:B27"/>
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="C49:C52"/>
     <mergeCell ref="C28:C33"/>
     <mergeCell ref="C34:C48"/>
     <mergeCell ref="B28:B52"/>
     <mergeCell ref="C13:C22"/>
     <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="B3:B27"/>
-    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
-    <hyperlink ref="E16" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E10" r:id="rId5"/>
-    <hyperlink ref="E15" r:id="rId6"/>
-    <hyperlink ref="E17" r:id="rId7"/>
-    <hyperlink ref="E19" r:id="rId8"/>
-    <hyperlink ref="E20" r:id="rId9"/>
-    <hyperlink ref="E24" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11"/>
-    <hyperlink ref="E8" r:id="rId12"/>
-    <hyperlink ref="E4" r:id="rId13"/>
-    <hyperlink ref="E18" r:id="rId14"/>
-    <hyperlink ref="E6" r:id="rId15"/>
-    <hyperlink ref="E5" r:id="rId16"/>
-    <hyperlink ref="E21" r:id="rId17"/>
-    <hyperlink ref="E22" r:id="rId18"/>
-    <hyperlink ref="E12" r:id="rId19"/>
-    <hyperlink ref="E26" r:id="rId20"/>
-    <hyperlink ref="E13" r:id="rId21"/>
-    <hyperlink ref="E11" r:id="rId22"/>
-    <hyperlink ref="E23" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E27" r:id="rId25"/>
-    <hyperlink ref="E49" r:id="rId26"/>
-    <hyperlink ref="E50" r:id="rId27"/>
-    <hyperlink ref="E51" r:id="rId28"/>
-    <hyperlink ref="E52" r:id="rId29"/>
-    <hyperlink ref="E28" r:id="rId30"/>
-    <hyperlink ref="E30" r:id="rId31"/>
-    <hyperlink ref="E31" r:id="rId32"/>
-    <hyperlink ref="E32" r:id="rId33"/>
-    <hyperlink ref="E29" r:id="rId34"/>
-    <hyperlink ref="E33" r:id="rId35"/>
-    <hyperlink ref="E34" r:id="rId36"/>
-    <hyperlink ref="E36" r:id="rId37"/>
-    <hyperlink ref="E37" r:id="rId38"/>
-    <hyperlink ref="E43" r:id="rId39"/>
-    <hyperlink ref="E45" r:id="rId40"/>
-    <hyperlink ref="E35" r:id="rId41"/>
-    <hyperlink ref="E38" r:id="rId42"/>
-    <hyperlink ref="E39" r:id="rId43"/>
-    <hyperlink ref="E40" r:id="rId44"/>
-    <hyperlink ref="E41" r:id="rId45"/>
-    <hyperlink ref="E42" r:id="rId46"/>
-    <hyperlink ref="E44" r:id="rId47"/>
-    <hyperlink ref="E46" r:id="rId48"/>
-    <hyperlink ref="E47" r:id="rId49"/>
-    <hyperlink ref="E48" r:id="rId50"/>
-    <hyperlink ref="E53" r:id="rId51"/>
-    <hyperlink ref="E54" r:id="rId52"/>
-    <hyperlink ref="E55" r:id="rId53"/>
-    <hyperlink ref="E56" r:id="rId54"/>
-    <hyperlink ref="E57" r:id="rId55"/>
-    <hyperlink ref="E58" r:id="rId56"/>
-    <hyperlink ref="E59" r:id="rId57"/>
-    <hyperlink ref="E60" r:id="rId58"/>
-    <hyperlink ref="E61" r:id="rId59"/>
-    <hyperlink ref="E62" r:id="rId60"/>
-    <hyperlink ref="E63" r:id="rId61"/>
-    <hyperlink ref="E64" r:id="rId62"/>
-    <hyperlink ref="E65" r:id="rId63"/>
-    <hyperlink ref="E66" r:id="rId64"/>
-    <hyperlink ref="E67" r:id="rId65"/>
-    <hyperlink ref="E68" r:id="rId66"/>
-    <hyperlink ref="E69" r:id="rId67"/>
-    <hyperlink ref="E70" r:id="rId68"/>
-    <hyperlink ref="E71" r:id="rId69"/>
-    <hyperlink ref="E72" r:id="rId70"/>
-    <hyperlink ref="E73" r:id="rId71"/>
-    <hyperlink ref="E74" r:id="rId72"/>
-    <hyperlink ref="E75" r:id="rId73"/>
-    <hyperlink ref="E76" r:id="rId74"/>
-    <hyperlink ref="E77" r:id="rId75"/>
-    <hyperlink ref="E78" r:id="rId76"/>
-    <hyperlink ref="E79" r:id="rId77"/>
-    <hyperlink ref="E80" r:id="rId78"/>
-    <hyperlink ref="E81" r:id="rId79"/>
-    <hyperlink ref="E82" r:id="rId80"/>
-    <hyperlink ref="E83" r:id="rId81"/>
-    <hyperlink ref="E84" r:id="rId82"/>
-    <hyperlink ref="E85" r:id="rId83"/>
-    <hyperlink ref="E86" r:id="rId84"/>
-    <hyperlink ref="E87" r:id="rId85"/>
-    <hyperlink ref="E88" r:id="rId86"/>
-    <hyperlink ref="E89" r:id="rId87"/>
-    <hyperlink ref="E90" r:id="rId88"/>
-    <hyperlink ref="E94" r:id="rId89"/>
-    <hyperlink ref="E91" r:id="rId90"/>
-    <hyperlink ref="E92" r:id="rId91"/>
-    <hyperlink ref="E93" r:id="rId92"/>
-    <hyperlink ref="E95" r:id="rId93"/>
-    <hyperlink ref="E96" r:id="rId94"/>
-    <hyperlink ref="E97" r:id="rId95"/>
-    <hyperlink ref="E98" r:id="rId96"/>
-    <hyperlink ref="E99" r:id="rId97"/>
-    <hyperlink ref="E100" r:id="rId98"/>
-    <hyperlink ref="E101" r:id="rId99"/>
-    <hyperlink ref="E102" r:id="rId100"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E24" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E13" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E49" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E50" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E51" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E52" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E28" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E30" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E31" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E32" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E29" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E33" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E34" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E45" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E35" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E38" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E39" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E40" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E41" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E42" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E44" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E46" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E47" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E48" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="E60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="E62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="E66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="E67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="E68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="E69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="E70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="E71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="E72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="E74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="E75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="E76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="E77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="E78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="E79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="E80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="E81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="E82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="E83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="E84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="E86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="E88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="E90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E94" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="E91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="E93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="E100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="E101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="E102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Site updated: 2020-06-23 15:45:01
</commit_message>
<xml_diff>
--- a/2020/06/15/2020春招-FLAG面试频率最高的100道题/2020春招-FLAG面试频率最高的100道题.xlsx
+++ b/2020/06/15/2020春招-FLAG面试频率最高的100道题/2020春招-FLAG面试频率最高的100道题.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1644b6d277bbd0f5/文档/Louis' Blog/source/_drafts/2020春招-FLAG面试频率最高的100道题/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_247634D3317F434A46BAEF313E0FE89AAB6DB088" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C53E01A2-4EC9-466C-AA44-2A9BB7F2BFC8}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_247634D3317F434A46BAEF313E0FE89AAB6DB088" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE2C1AD1-D876-4A4E-B5EA-186E6364086D}"/>
   <bookViews>
     <workbookView xWindow="2168" yWindow="1868" windowWidth="15389" windowHeight="9644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,7 +826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,6 +848,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +890,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -918,10 +924,13 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -930,8 +939,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1219,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1234,12 +1243,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="41.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -1258,10 +1267,10 @@
     </row>
     <row r="3" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1273,8 +1282,8 @@
     </row>
     <row r="4" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="10" t="s">
         <v>33</v>
       </c>
@@ -1284,8 +1293,8 @@
     </row>
     <row r="5" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
@@ -1295,8 +1304,8 @@
     </row>
     <row r="6" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="10" t="s">
         <v>37</v>
       </c>
@@ -1306,8 +1315,8 @@
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1317,8 +1326,8 @@
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="10" t="s">
         <v>31</v>
       </c>
@@ -1328,8 +1337,8 @@
     </row>
     <row r="9" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
@@ -1339,8 +1348,8 @@
     </row>
     <row r="10" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
@@ -1350,8 +1359,8 @@
     </row>
     <row r="11" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="10" t="s">
         <v>51</v>
       </c>
@@ -1361,8 +1370,8 @@
     </row>
     <row r="12" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="10" t="s">
         <v>45</v>
       </c>
@@ -1372,8 +1381,8 @@
     </row>
     <row r="13" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1385,8 +1394,8 @@
     </row>
     <row r="14" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="10" t="s">
         <v>29</v>
       </c>
@@ -1396,9 +1405,9 @@
     </row>
     <row r="15" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="5" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="7" t="s">
@@ -1407,9 +1416,9 @@
     </row>
     <row r="16" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="6" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1418,9 +1427,9 @@
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="10" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1429,9 +1438,9 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -1440,8 +1449,8 @@
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1451,8 +1460,8 @@
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="6" t="s">
         <v>24</v>
       </c>
@@ -1462,8 +1471,8 @@
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="6" t="s">
         <v>41</v>
       </c>
@@ -1473,8 +1482,8 @@
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="13"/>
       <c r="D22" s="6" t="s">
         <v>43</v>
       </c>
@@ -1484,8 +1493,8 @@
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1497,8 +1506,8 @@
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="6" t="s">
         <v>26</v>
       </c>
@@ -1508,8 +1517,8 @@
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="5" t="s">
         <v>54</v>
       </c>
@@ -1519,8 +1528,8 @@
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="5" t="s">
         <v>47</v>
       </c>
@@ -1530,8 +1539,8 @@
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="5" t="s">
         <v>55</v>
       </c>
@@ -1541,10 +1550,10 @@
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1555,8 +1564,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B29" s="12"/>
-      <c r="C29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="4" t="s">
         <v>58</v>
       </c>
@@ -1565,8 +1574,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B30" s="12"/>
-      <c r="C30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1575,8 +1584,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B31" s="12"/>
-      <c r="C31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="5" t="s">
         <v>60</v>
       </c>
@@ -1585,8 +1594,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B32" s="12"/>
-      <c r="C32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="5" t="s">
         <v>61</v>
       </c>
@@ -1595,8 +1604,8 @@
       </c>
     </row>
     <row r="33" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B33" s="12"/>
-      <c r="C33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="5" t="s">
         <v>66</v>
       </c>
@@ -1605,8 +1614,8 @@
       </c>
     </row>
     <row r="34" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
-      <c r="C34" s="15" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -1617,8 +1626,8 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="12"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="6" t="s">
         <v>68</v>
       </c>
@@ -1627,8 +1636,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B36" s="12"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="5" t="s">
         <v>69</v>
       </c>
@@ -1637,8 +1646,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
-      <c r="C37" s="15"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="6" t="s">
         <v>70</v>
       </c>
@@ -1647,8 +1656,8 @@
       </c>
     </row>
     <row r="38" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B38" s="12"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="13"/>
       <c r="D38" s="6" t="s">
         <v>71</v>
       </c>
@@ -1657,8 +1666,8 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B39" s="12"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="13"/>
       <c r="D39" s="5" t="s">
         <v>72</v>
       </c>
@@ -1667,8 +1676,8 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B40" s="12"/>
-      <c r="C40" s="15"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="6" t="s">
         <v>73</v>
       </c>
@@ -1677,8 +1686,8 @@
       </c>
     </row>
     <row r="41" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
-      <c r="C41" s="15"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="13"/>
       <c r="D41" s="6" t="s">
         <v>74</v>
       </c>
@@ -1687,8 +1696,8 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B42" s="12"/>
-      <c r="C42" s="15"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="6" t="s">
         <v>75</v>
       </c>
@@ -1697,8 +1706,8 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B43" s="12"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="6" t="s">
         <v>76</v>
       </c>
@@ -1707,8 +1716,8 @@
       </c>
     </row>
     <row r="44" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B44" s="12"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="6" t="s">
         <v>77</v>
       </c>
@@ -1717,8 +1726,8 @@
       </c>
     </row>
     <row r="45" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B45" s="12"/>
-      <c r="C45" s="15"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="6" t="s">
         <v>78</v>
       </c>
@@ -1727,8 +1736,8 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B46" s="12"/>
-      <c r="C46" s="15"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="5" t="s">
         <v>79</v>
       </c>
@@ -1737,8 +1746,8 @@
       </c>
     </row>
     <row r="47" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B47" s="12"/>
-      <c r="C47" s="15"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="5" t="s">
         <v>80</v>
       </c>
@@ -1747,8 +1756,8 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B48" s="12"/>
-      <c r="C48" s="15"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="5" t="s">
         <v>81</v>
       </c>
@@ -1757,8 +1766,8 @@
       </c>
     </row>
     <row r="49" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B49" s="12"/>
-      <c r="C49" s="11" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -1769,8 +1778,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B50" s="12"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="12"/>
       <c r="D50" s="6" t="s">
         <v>84</v>
       </c>
@@ -1779,8 +1788,8 @@
       </c>
     </row>
     <row r="51" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B51" s="12"/>
-      <c r="C51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
       <c r="D51" s="5" t="s">
         <v>86</v>
       </c>
@@ -1789,8 +1798,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B52" s="12"/>
-      <c r="C52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="5" t="s">
         <v>88</v>
       </c>
@@ -1799,10 +1808,10 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -1813,8 +1822,8 @@
       </c>
     </row>
     <row r="54" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B54" s="12"/>
-      <c r="C54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="4" t="s">
         <v>114</v>
       </c>
@@ -1823,8 +1832,8 @@
       </c>
     </row>
     <row r="55" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B55" s="12"/>
-      <c r="C55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="5" t="s">
         <v>116</v>
       </c>
@@ -1833,8 +1842,8 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B56" s="12"/>
-      <c r="C56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="6" t="s">
         <v>118</v>
       </c>
@@ -1843,8 +1852,8 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B57" s="12"/>
-      <c r="C57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="6" t="s">
         <v>120</v>
       </c>
@@ -1853,8 +1862,8 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B58" s="12"/>
-      <c r="C58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="5" t="s">
         <v>122</v>
       </c>
@@ -1863,8 +1872,8 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B59" s="12"/>
-      <c r="C59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="6" t="s">
         <v>58</v>
       </c>
@@ -1873,8 +1882,8 @@
       </c>
     </row>
     <row r="60" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B60" s="12"/>
-      <c r="C60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="6" t="s">
         <v>124</v>
       </c>
@@ -1883,8 +1892,8 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B61" s="12"/>
-      <c r="C61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="5" t="s">
         <v>126</v>
       </c>
@@ -1893,8 +1902,8 @@
       </c>
     </row>
     <row r="62" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B62" s="12"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="5" t="s">
         <v>128</v>
       </c>
@@ -1903,8 +1912,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B63" s="12"/>
-      <c r="C63" s="15" t="s">
+      <c r="B63" s="11"/>
+      <c r="C63" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="6" t="s">
@@ -1915,8 +1924,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B64" s="12"/>
-      <c r="C64" s="15"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="13"/>
       <c r="D64" s="6" t="s">
         <v>132</v>
       </c>
@@ -1925,8 +1934,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B65" s="12"/>
-      <c r="C65" s="15"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="13"/>
       <c r="D65" s="5" t="s">
         <v>134</v>
       </c>
@@ -1935,8 +1944,8 @@
       </c>
     </row>
     <row r="66" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B66" s="12"/>
-      <c r="C66" s="15"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="13"/>
       <c r="D66" s="6" t="s">
         <v>136</v>
       </c>
@@ -1945,8 +1954,8 @@
       </c>
     </row>
     <row r="67" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B67" s="12"/>
-      <c r="C67" s="15"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="13"/>
       <c r="D67" s="6" t="s">
         <v>138</v>
       </c>
@@ -1955,8 +1964,8 @@
       </c>
     </row>
     <row r="68" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B68" s="12"/>
-      <c r="C68" s="15"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="13"/>
       <c r="D68" s="5" t="s">
         <v>140</v>
       </c>
@@ -1965,8 +1974,8 @@
       </c>
     </row>
     <row r="69" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B69" s="12"/>
-      <c r="C69" s="15"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="13"/>
       <c r="D69" s="6" t="s">
         <v>142</v>
       </c>
@@ -1975,8 +1984,8 @@
       </c>
     </row>
     <row r="70" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B70" s="12"/>
-      <c r="C70" s="15"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="13"/>
       <c r="D70" s="6" t="s">
         <v>144</v>
       </c>
@@ -1985,8 +1994,8 @@
       </c>
     </row>
     <row r="71" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B71" s="12"/>
-      <c r="C71" s="15"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="6" t="s">
         <v>146</v>
       </c>
@@ -1995,8 +2004,8 @@
       </c>
     </row>
     <row r="72" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B72" s="12"/>
-      <c r="C72" s="15"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="13"/>
       <c r="D72" s="6" t="s">
         <v>148</v>
       </c>
@@ -2005,8 +2014,8 @@
       </c>
     </row>
     <row r="73" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B73" s="12"/>
-      <c r="C73" s="11" t="s">
+      <c r="B73" s="11"/>
+      <c r="C73" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D73" s="6" t="s">
@@ -2017,8 +2026,8 @@
       </c>
     </row>
     <row r="74" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B74" s="12"/>
-      <c r="C74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="6" t="s">
         <v>152</v>
       </c>
@@ -2027,8 +2036,8 @@
       </c>
     </row>
     <row r="75" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B75" s="12"/>
-      <c r="C75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="12"/>
       <c r="D75" s="5" t="s">
         <v>153</v>
       </c>
@@ -2037,8 +2046,8 @@
       </c>
     </row>
     <row r="76" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B76" s="12"/>
-      <c r="C76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="12"/>
       <c r="D76" s="5" t="s">
         <v>155</v>
       </c>
@@ -2047,8 +2056,8 @@
       </c>
     </row>
     <row r="77" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B77" s="12"/>
-      <c r="C77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="5" t="s">
         <v>157</v>
       </c>
@@ -2057,10 +2066,10 @@
       </c>
     </row>
     <row r="78" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -2071,8 +2080,8 @@
       </c>
     </row>
     <row r="79" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B79" s="12"/>
-      <c r="C79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
       <c r="D79" s="4" t="s">
         <v>114</v>
       </c>
@@ -2081,8 +2090,8 @@
       </c>
     </row>
     <row r="80" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B80" s="12"/>
-      <c r="C80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
       <c r="D80" s="5" t="s">
         <v>39</v>
       </c>
@@ -2091,8 +2100,8 @@
       </c>
     </row>
     <row r="81" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B81" s="12"/>
-      <c r="C81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12"/>
       <c r="D81" s="6" t="s">
         <v>62</v>
       </c>
@@ -2101,8 +2110,8 @@
       </c>
     </row>
     <row r="82" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B82" s="12"/>
-      <c r="C82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="12"/>
       <c r="D82" s="6" t="s">
         <v>124</v>
       </c>
@@ -2111,8 +2120,8 @@
       </c>
     </row>
     <row r="83" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B83" s="12"/>
-      <c r="C83" s="15" t="s">
+      <c r="B83" s="11"/>
+      <c r="C83" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D83" s="6" t="s">
@@ -2123,8 +2132,8 @@
       </c>
     </row>
     <row r="84" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B84" s="12"/>
-      <c r="C84" s="15"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="13"/>
       <c r="D84" s="6" t="s">
         <v>130</v>
       </c>
@@ -2133,8 +2142,8 @@
       </c>
     </row>
     <row r="85" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B85" s="12"/>
-      <c r="C85" s="15"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="13"/>
       <c r="D85" s="5" t="s">
         <v>134</v>
       </c>
@@ -2143,8 +2152,8 @@
       </c>
     </row>
     <row r="86" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B86" s="12"/>
-      <c r="C86" s="15"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="13"/>
       <c r="D86" s="6" t="s">
         <v>166</v>
       </c>
@@ -2153,8 +2162,8 @@
       </c>
     </row>
     <row r="87" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B87" s="12"/>
-      <c r="C87" s="15"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="13"/>
       <c r="D87" s="6" t="s">
         <v>168</v>
       </c>
@@ -2163,8 +2172,8 @@
       </c>
     </row>
     <row r="88" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B88" s="12"/>
-      <c r="C88" s="15"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="13"/>
       <c r="D88" s="5" t="s">
         <v>170</v>
       </c>
@@ -2173,8 +2182,8 @@
       </c>
     </row>
     <row r="89" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B89" s="12"/>
-      <c r="C89" s="15"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="13"/>
       <c r="D89" s="6" t="s">
         <v>142</v>
       </c>
@@ -2183,8 +2192,8 @@
       </c>
     </row>
     <row r="90" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B90" s="12"/>
-      <c r="C90" s="15"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="13"/>
       <c r="D90" s="6" t="s">
         <v>172</v>
       </c>
@@ -2193,8 +2202,8 @@
       </c>
     </row>
     <row r="91" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B91" s="12"/>
-      <c r="C91" s="15"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="13"/>
       <c r="D91" s="6" t="s">
         <v>176</v>
       </c>
@@ -2203,8 +2212,8 @@
       </c>
     </row>
     <row r="92" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B92" s="12"/>
-      <c r="C92" s="15"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="13"/>
       <c r="D92" s="6" t="s">
         <v>178</v>
       </c>
@@ -2213,8 +2222,8 @@
       </c>
     </row>
     <row r="93" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B93" s="12"/>
-      <c r="C93" s="15"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="13"/>
       <c r="D93" s="5" t="s">
         <v>180</v>
       </c>
@@ -2223,8 +2232,8 @@
       </c>
     </row>
     <row r="94" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B94" s="12"/>
-      <c r="C94" s="15"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="13"/>
       <c r="D94" s="6" t="s">
         <v>174</v>
       </c>
@@ -2233,8 +2242,8 @@
       </c>
     </row>
     <row r="95" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B95" s="12"/>
-      <c r="C95" s="15"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="13"/>
       <c r="D95" s="6" t="s">
         <v>182</v>
       </c>
@@ -2243,8 +2252,8 @@
       </c>
     </row>
     <row r="96" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B96" s="12"/>
-      <c r="C96" s="15"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="13"/>
       <c r="D96" s="6" t="s">
         <v>184</v>
       </c>
@@ -2253,8 +2262,8 @@
       </c>
     </row>
     <row r="97" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B97" s="12"/>
-      <c r="C97" s="15"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="13"/>
       <c r="D97" s="5" t="s">
         <v>186</v>
       </c>
@@ -2263,8 +2272,8 @@
       </c>
     </row>
     <row r="98" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B98" s="12"/>
-      <c r="C98" s="11" t="s">
+      <c r="B98" s="11"/>
+      <c r="C98" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D98" s="6" t="s">
@@ -2275,8 +2284,8 @@
       </c>
     </row>
     <row r="99" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B99" s="12"/>
-      <c r="C99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="12"/>
       <c r="D99" s="6" t="s">
         <v>188</v>
       </c>
@@ -2285,8 +2294,8 @@
       </c>
     </row>
     <row r="100" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B100" s="12"/>
-      <c r="C100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="12"/>
       <c r="D100" s="5" t="s">
         <v>190</v>
       </c>
@@ -2295,8 +2304,8 @@
       </c>
     </row>
     <row r="101" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B101" s="12"/>
-      <c r="C101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="12"/>
       <c r="D101" s="5" t="s">
         <v>192</v>
       </c>
@@ -2305,8 +2314,8 @@
       </c>
     </row>
     <row r="102" spans="2:5" ht="17.649999999999999" x14ac:dyDescent="0.3">
-      <c r="B102" s="12"/>
-      <c r="C102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="12"/>
       <c r="D102" s="5" t="s">
         <v>195</v>
       </c>
@@ -2316,14 +2325,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B53:B77"/>
-    <mergeCell ref="C53:C62"/>
-    <mergeCell ref="C63:C72"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="B78:B102"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C97"/>
-    <mergeCell ref="C98:C102"/>
     <mergeCell ref="C3:C12"/>
     <mergeCell ref="B3:B27"/>
     <mergeCell ref="B1:E1"/>
@@ -2333,6 +2334,14 @@
     <mergeCell ref="B28:B52"/>
     <mergeCell ref="C13:C22"/>
     <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B53:B77"/>
+    <mergeCell ref="C53:C62"/>
+    <mergeCell ref="C63:C72"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="B78:B102"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C97"/>
+    <mergeCell ref="C98:C102"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>